<commit_message>
add ontology IDs to tags
</commit_message>
<xml_diff>
--- a/templates/dataplant/GEO/GEO_-_High-throughput_sequencing_-_Computational_analysis.xlsx
+++ b/templates/dataplant/GEO/GEO_-_High-throughput_sequencing_-_Computational_analysis.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Transcriptomics</t>
   </si>
   <si>
-    <t>Computational Analysis</t>
-  </si>
-  <si>
     <t>mandatory</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C47925</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C61298</t>
   </si>
   <si>
     <t>Tags Term Source REF</t>
@@ -732,17 +732,20 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>29</v>
       </c>
       <c r="F14" t="s">
@@ -752,6 +755,9 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
       </c>
       <c r="F15" t="s">
         <v>32</v>

</xml_diff>